<commit_message>
Pequeños cambios no terminados
</commit_message>
<xml_diff>
--- a/Doo-Doc/Nueva Version Victus/MuestreoDatos/ConjuntosResidenciales Muestro Datos.xlsx
+++ b/Doo-Doc/Nueva Version Victus/MuestreoDatos/ConjuntosResidenciales Muestro Datos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Music\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uconet-my.sharepoint.com/personal/juan_avendano1956_uco_net_co/Documents/Documents/victus-doc/Doo-Doc/Nueva Version Victus/MuestreoDatos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74AB84A-B165-41E5-BAD9-CF6557DE9E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{D74AB84A-B165-41E5-BAD9-CF6557DE9E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8869C936-CE84-42A3-89AD-9281A90F1BBF}"/>
   <bookViews>
-    <workbookView xWindow="15855" yWindow="1725" windowWidth="20220" windowHeight="15345" activeTab="5" xr2:uid="{46B52760-6E94-4759-BDEF-A2400BC5A0BB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{46B52760-6E94-4759-BDEF-A2400BC5A0BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Objetos de dominio" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="83">
   <si>
     <t>Nombre</t>
   </si>
@@ -97,9 +97,6 @@
     <t>Es un dato que representa el formato de texto de una dirección.</t>
   </si>
   <si>
-    <t>Es un dato que representa el número de contacto de una conjunto residencial</t>
-  </si>
-  <si>
     <t>Es un dato que representa la descripción que tiene el conjunto residencial para ser identificado con palabras.</t>
   </si>
   <si>
@@ -139,9 +136,6 @@
     <t>Usar la maquinaria con toalla y mantener la higiene</t>
   </si>
   <si>
-    <t>No puede haber más de un administrador con el mismo correo electrónico.</t>
-  </si>
-  <si>
     <t>Es un dato que representa al nombre de una zona comun.</t>
   </si>
   <si>
@@ -208,12 +202,6 @@
     <t>sara@gmail.com</t>
   </si>
   <si>
-    <t>Carlos-carlos@gmail.com</t>
-  </si>
-  <si>
-    <t>Sara-sara@gmail.com</t>
-  </si>
-  <si>
     <t>tipoZonaInmueble</t>
   </si>
   <si>
@@ -229,9 +217,6 @@
     <t>ZonaInmueble</t>
   </si>
   <si>
-    <t>Capacidad</t>
-  </si>
-  <si>
     <t>Inmueble</t>
   </si>
   <si>
@@ -262,16 +247,49 @@
     <t>Es un dato que representa cuantos minutos son permitidos por uso en un dia la zona común</t>
   </si>
   <si>
-    <t>tiempoUso</t>
-  </si>
-  <si>
-    <t>unidadDeTiempoUso</t>
-  </si>
-  <si>
     <t>Minutos</t>
   </si>
   <si>
     <t>Hora</t>
+  </si>
+  <si>
+    <t>Capacidad de personas</t>
+  </si>
+  <si>
+    <t>tiempo de uso</t>
+  </si>
+  <si>
+    <t>Unidad de tiempo de uso</t>
+  </si>
+  <si>
+    <t>No puede haber más de un administrador con el mismo correo electrónico y el mismo numero de contacto.</t>
+  </si>
+  <si>
+    <t>Ciudad</t>
+  </si>
+  <si>
+    <t>Departamento</t>
+  </si>
+  <si>
+    <t>Rionegro</t>
+  </si>
+  <si>
+    <t>Antioquia</t>
+  </si>
+  <si>
+    <t>Medellín</t>
+  </si>
+  <si>
+    <t>Contacto de portería</t>
+  </si>
+  <si>
+    <t>Es un dato que representa el número de contacto de la portería de una conjunto residencial</t>
+  </si>
+  <si>
+    <t>Es un dato que representa el municipio dónde se encuentra un conjunto residencial.</t>
+  </si>
+  <si>
+    <t>Es un dato que representa el departamento dónde se encuentra el conjunto residencial.</t>
   </si>
 </sst>
 </file>
@@ -421,9 +439,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -445,9 +460,12 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -464,7 +482,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -786,13 +804,13 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="2" width="58.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="58.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -800,15 +818,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -816,28 +834,28 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -857,45 +875,45 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="23.85546875" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" customWidth="1"/>
-    <col min="7" max="7" width="33" customWidth="1"/>
+    <col min="6" max="6" width="23.88671875" customWidth="1"/>
+    <col min="7" max="7" width="38.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -903,70 +921,70 @@
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>1</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D4" s="12">
         <v>3053456459</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F4" s="12">
         <v>123456</v>
       </c>
       <c r="G4" s="13" t="str">
-        <f>B4&amp;"-"&amp;E4</f>
-        <v>Carlos-carlos@gmail.com</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <f>B4&amp;"-"&amp;D4&amp;"-"&amp;E4</f>
+        <v>Carlos-3053456459-carlos@gmail.com</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>2</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D5" s="1">
         <v>3584418688</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F5" s="1">
         <v>654321</v>
       </c>
       <c r="G5" s="13" t="str">
-        <f t="shared" ref="G5:G6" si="0">B5&amp;"-"&amp;E5</f>
-        <v>Sara-sara@gmail.com</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" ref="G5:G6" si="0">B5&amp;"-"&amp;D5&amp;"-"&amp;E5</f>
+        <v>Sara-3584418688-sara@gmail.com</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -977,7 +995,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>--</v>
       </c>
     </row>
   </sheetData>
@@ -996,31 +1014,33 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CCBB1F3-C6CB-4282-9EE1-3BEE3EA280EE}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="21.7109375" customWidth="1"/>
-    <col min="5" max="6" width="36" customWidth="1"/>
-    <col min="7" max="7" width="29" customWidth="1"/>
+    <col min="2" max="6" width="21.6640625" customWidth="1"/>
+    <col min="7" max="8" width="36" customWidth="1"/>
+    <col min="9" max="9" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
       <c r="G1" s="6"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>15</v>
       </c>
@@ -1031,17 +1051,23 @@
         <v>17</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="7"/>
+      <c r="I2" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1052,19 +1078,25 @@
         <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="I3" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -1074,56 +1106,70 @@
       <c r="C4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="9">
         <v>3053451564</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="10" t="str">
+      <c r="H4" s="24" t="str">
+        <f>Administrador!G4</f>
+        <v>Carlos-3053456459-carlos@gmail.com</v>
+      </c>
+      <c r="I4" s="10" t="str">
         <f>_xlfn.CONCAT(A4,"-",B4)</f>
         <v>1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>2</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F5" s="9">
+        <v>3057477789</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="9">
-        <v>3057477789</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" s="10" t="str">
+      <c r="H5" s="24" t="str">
+        <f>Administrador!G5</f>
+        <v>Sara-3584418688-sara@gmail.com</v>
+      </c>
+      <c r="I5" s="10" t="str">
         <f>_xlfn.CONCAT(A5,"-",B5)</f>
         <v>2-Natural</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A1" location="Objetos de dominio!A1" display="Objetos de dominio!A1" xr:uid="{D64C3258-0F3E-431B-9317-C8728CDAC55D}"/>
-    <hyperlink ref="G1" location="Objetos de dominio!A1" display="Objetos de dominio!A1" xr:uid="{AFF80FE2-F73C-488E-9508-D9E1A9B6135D}"/>
-    <hyperlink ref="F4" location="Administrador!A4" display="Carlos-carlos@gmail.com" xr:uid="{7D168C2A-3F1A-4D3F-A05A-5350E0C9CC3B}"/>
-    <hyperlink ref="F5" location="Administrador!A5" display="Sara-sara@gmail.com" xr:uid="{DC6D880C-E01A-4A61-9B2D-31FCC8E19585}"/>
-    <hyperlink ref="A1:D1" location="'Objetos de dominio'!A1" display="&lt;&lt;&lt;&lt;&lt;&lt; Volver al inicio" xr:uid="{E47C9477-04BF-4359-AA4E-108F5F557D82}"/>
-    <hyperlink ref="F3" location="Administrador!A1" display="Administrador" xr:uid="{8573C9AA-E4AB-4C12-80E7-A396F426EDA8}"/>
+    <hyperlink ref="I1" location="Objetos de dominio!A1" display="Objetos de dominio!A1" xr:uid="{AFF80FE2-F73C-488E-9508-D9E1A9B6135D}"/>
+    <hyperlink ref="H4" location="Administrador!A4" display="Carlos-carlos@gmail.com" xr:uid="{7D168C2A-3F1A-4D3F-A05A-5350E0C9CC3B}"/>
+    <hyperlink ref="A1:F1" location="'Objetos de dominio'!A1" display="&lt;&lt;&lt;&lt;&lt;&lt; Volver al inicio" xr:uid="{E47C9477-04BF-4359-AA4E-108F5F557D82}"/>
+    <hyperlink ref="H3" location="Administrador!A1" display="Administrador" xr:uid="{8573C9AA-E4AB-4C12-80E7-A396F426EDA8}"/>
+    <hyperlink ref="H5" location="Administrador!A4" display="Carlos-carlos@gmail.com" xr:uid="{B691C4A3-C438-46E2-9139-486F3E66B20C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1133,53 +1179,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{615584B6-BB9C-4024-AABA-069882FFA83A}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" customWidth="1"/>
-    <col min="5" max="5" width="37.140625" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" customWidth="1"/>
+    <col min="5" max="5" width="37.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>2</v>
@@ -1188,72 +1234,72 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>1</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E4" s="10" t="str">
         <f>_xlfn.CONCAT(B4,C4," de ",D4)</f>
         <v>Torre1 de 1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E5" s="10" t="str">
         <f t="shared" ref="E5:E12" si="0">_xlfn.CONCAT(B5,C5," de ",D5)</f>
         <v>Bloque1 de 1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E6" s="10" t="str">
         <f t="shared" si="0"/>
         <v>Torre2 de 1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>4</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
       </c>
       <c r="D7" s="3" t="str">
-        <f>ConjuntoResidencial!$G$5</f>
+        <f>ConjuntoResidencial!$I$5</f>
         <v>2-Natural</v>
       </c>
       <c r="E7" s="10" t="str">
@@ -1261,19 +1307,26 @@
         <v>Bloque2 de 2-Natural</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="B8" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1" t="str">
+        <f>ConjuntoResidencial!I4</f>
+        <v>1-Forest apartamentos</v>
+      </c>
       <c r="E8" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> de </v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>Bloque4 de 1-Forest apartamentos</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -1285,7 +1338,7 @@
         <v xml:space="preserve"> de </v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -1297,7 +1350,7 @@
         <v xml:space="preserve"> de </v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -1309,7 +1362,7 @@
         <v xml:space="preserve"> de </v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -1321,14 +1374,14 @@
         <v xml:space="preserve"> de </v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1361,63 +1414,63 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="31.42578125" customWidth="1"/>
-    <col min="5" max="5" width="49.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="31.44140625" customWidth="1"/>
+    <col min="5" max="5" width="49.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>1</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C4" s="1">
         <v>102</v>
@@ -1431,12 +1484,12 @@
         <v>Apartamento '102' de Torre1 de 1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C5" s="1">
         <v>10</v>
@@ -1450,12 +1503,12 @@
         <v>Casa '10' de Bloque1 de 1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C6" s="1">
         <v>304</v>
@@ -1469,12 +1522,12 @@
         <v>Apartamento '304' de Torre2 de 1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>4</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C7" s="1">
         <v>11</v>
@@ -1488,7 +1541,7 @@
         <v>Casa '11' de Bloque2 de 2-Natural</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -1500,7 +1553,7 @@
         <v xml:space="preserve"> '' de </v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -1512,7 +1565,7 @@
         <v xml:space="preserve"> '' de </v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -1524,14 +1577,14 @@
         <v xml:space="preserve"> '' de </v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1560,22 +1613,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F3E3BD9-49ED-471B-BA3A-A84E923CE558}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="7" width="21.7109375" customWidth="1"/>
+    <col min="5" max="7" width="21.6640625" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="23.7109375" customWidth="1"/>
-    <col min="10" max="10" width="33.140625" customWidth="1"/>
+    <col min="9" max="9" width="23.6640625" customWidth="1"/>
+    <col min="10" max="10" width="33.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
@@ -1589,37 +1642,37 @@
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>36</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1627,22 +1680,22 @@
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>2</v>
@@ -1651,31 +1704,31 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="16">
+    <row r="4" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="15">
         <v>1</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="19">
+      <c r="C4" s="16"/>
+      <c r="D4" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="18">
         <v>50</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="18">
         <v>60</v>
       </c>
-      <c r="G4" s="19" t="s">
-        <v>75</v>
+      <c r="G4" s="18" t="s">
+        <v>68</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I4" s="3" t="str">
-        <f>ConjuntoResidencial!$G$4</f>
+        <f>ConjuntoResidencial!$I$4</f>
         <v>1-Forest apartamentos</v>
       </c>
       <c r="J4" s="10" t="str">
@@ -1683,31 +1736,31 @@
         <v>Piscina-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="84" x14ac:dyDescent="0.35">
-      <c r="A5" s="20">
+    <row r="5" spans="1:10" ht="84" x14ac:dyDescent="0.4">
+      <c r="A5" s="19">
         <v>2</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="21" t="s">
+      <c r="E5" s="21">
+        <v>20</v>
+      </c>
+      <c r="F5" s="21">
+        <v>120</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="22">
-        <v>20</v>
-      </c>
-      <c r="F5" s="22">
-        <v>120</v>
-      </c>
-      <c r="G5" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>31</v>
-      </c>
       <c r="I5" s="3" t="str">
-        <f>ConjuntoResidencial!$G$4</f>
+        <f>ConjuntoResidencial!$I$4</f>
         <v>1-Forest apartamentos</v>
       </c>
       <c r="J5" s="10" t="str">
@@ -1715,31 +1768,31 @@
         <v>Gimnasio-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="73.150000000000006" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="20">
+    <row r="6" spans="1:10" ht="73.2" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="19">
         <v>3</v>
       </c>
-      <c r="B6" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="22">
+      <c r="B6" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="19"/>
+      <c r="D6" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="21">
         <v>15</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="21">
         <v>1</v>
       </c>
-      <c r="G6" s="22" t="s">
-        <v>76</v>
+      <c r="G6" s="21" t="s">
+        <v>69</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I6" s="3" t="str">
-        <f>ConjuntoResidencial!$G$5</f>
+        <f>ConjuntoResidencial!$I$5</f>
         <v>2-Natural</v>
       </c>
       <c r="J6" s="10" t="str">

</xml_diff>

<commit_message>
Muestreo de datos agradando para conjuntos residenciales
</commit_message>
<xml_diff>
--- a/Doo-Doc/Nueva Version Victus/MuestreoDatos/ConjuntosResidenciales Muestro Datos.xlsx
+++ b/Doo-Doc/Nueva Version Victus/MuestreoDatos/ConjuntosResidenciales Muestro Datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uconet-my.sharepoint.com/personal/juan_avendano1956_uco_net_co/Documents/Documents/victus-doc/Doo-Doc/Nueva Version Victus/MuestreoDatos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{D74AB84A-B165-41E5-BAD9-CF6557DE9E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8869C936-CE84-42A3-89AD-9281A90F1BBF}"/>
+  <xr:revisionPtr revIDLastSave="226" documentId="13_ncr:1_{D74AB84A-B165-41E5-BAD9-CF6557DE9E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4E4A383-F6DE-41E5-8FA1-0D6CBFA2B71F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{46B52760-6E94-4759-BDEF-A2400BC5A0BB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{46B52760-6E94-4759-BDEF-A2400BC5A0BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Objetos de dominio" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="141">
   <si>
     <t>Nombre</t>
   </si>
@@ -196,9 +196,6 @@
     <t>Sanchez</t>
   </si>
   <si>
-    <t>carlos@gmail.com</t>
-  </si>
-  <si>
     <t>sara@gmail.com</t>
   </si>
   <si>
@@ -290,13 +287,190 @@
   </si>
   <si>
     <t>Es un dato que representa el departamento dónde se encuentra el conjunto residencial.</t>
+  </si>
+  <si>
+    <t>Riogrande</t>
+  </si>
+  <si>
+    <t>Bolivar</t>
+  </si>
+  <si>
+    <t>Ventus</t>
+  </si>
+  <si>
+    <t>Calle 45 # 12-34</t>
+  </si>
+  <si>
+    <t>Carrera 8 # 34-56</t>
+  </si>
+  <si>
+    <t>Avenida 9 # 7-89</t>
+  </si>
+  <si>
+    <t>Un conjunto cerrado con amplias zonas verdes y áreas recreativas para toda la familia.</t>
+  </si>
+  <si>
+    <t>Barranquilla</t>
+  </si>
+  <si>
+    <t>Atlántico</t>
+  </si>
+  <si>
+    <t>Un lugar tranquilo con seguridad las 24 horas y acceso a servicios cercanos.</t>
+  </si>
+  <si>
+    <t>Bogotá</t>
+  </si>
+  <si>
+    <t>Cundinamarca</t>
+  </si>
+  <si>
+    <t>Moderno conjunto residencial con gimnasio, piscina y salón de eventos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">María </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gonzales </t>
+  </si>
+  <si>
+    <t>maria.gonzalez@example.com</t>
+  </si>
+  <si>
+    <t>Mg67890@</t>
+  </si>
+  <si>
+    <t>fd654321</t>
+  </si>
+  <si>
+    <t>as123456</t>
+  </si>
+  <si>
+    <t>Laura</t>
+  </si>
+  <si>
+    <t>Martínez</t>
+  </si>
+  <si>
+    <t>laura.martinez@example.com</t>
+  </si>
+  <si>
+    <t>Lm34567$</t>
+  </si>
+  <si>
+    <t>Andrés</t>
+  </si>
+  <si>
+    <t>López</t>
+  </si>
+  <si>
+    <t>andres.lopez@example.com</t>
+  </si>
+  <si>
+    <t>carlos@example.com</t>
+  </si>
+  <si>
+    <t>Sofía</t>
+  </si>
+  <si>
+    <t>Torres</t>
+  </si>
+  <si>
+    <t>sofia.torres@example.com</t>
+  </si>
+  <si>
+    <t>St45678^</t>
+  </si>
+  <si>
+    <t>Al89012%</t>
+  </si>
+  <si>
+    <t>Salón de Eventos</t>
+  </si>
+  <si>
+    <t>Un espacio amplio para celebrar reuniones sociales y familiares.</t>
+  </si>
+  <si>
+    <t>Reservar con al menos 3 días de anticipación. No se permite el uso de pirotecnia.</t>
+  </si>
+  <si>
+    <t>Cancha de Fútbol</t>
+  </si>
+  <si>
+    <t>Cancha de césped sintético para actividades deportivas en equipo.</t>
+  </si>
+  <si>
+    <t>Se requiere reservar con 2 horas de anticipación. Uso exclusivo de zapatos con tacos adecuados.</t>
+  </si>
+  <si>
+    <t>Piscina Pequeña</t>
+  </si>
+  <si>
+    <t>Piscina diseñada para niños, con profundidades seguras y vigilancia.</t>
+  </si>
+  <si>
+    <t>Es necesario el acompañamiento de un adulto. No se permite correr alrededor de la piscina.</t>
+  </si>
+  <si>
+    <t>Zona BBQ</t>
+  </si>
+  <si>
+    <t>Área equipada con parrillas y mesas para realizar asados al aire libre.</t>
+  </si>
+  <si>
+    <t>Limpiar el área después de cada uso. Se debe reservar con 1 día de anticipación.</t>
+  </si>
+  <si>
+    <t>Cancha de Tenis</t>
+  </si>
+  <si>
+    <t>Espacio deportivo para la práctica de tenis en un ambiente profesional</t>
+  </si>
+  <si>
+    <t>Uso exclusivo de zapatos de suela lisa. Reservar con 4 horas de anticipación.</t>
+  </si>
+  <si>
+    <t>Sala de Juegos</t>
+  </si>
+  <si>
+    <t>Sala equipada con mesas de ping-pong, billar y juegos de mesa para el disfrute familiar.</t>
+  </si>
+  <si>
+    <t>Reservar con al menos 2 horas de anticipación. Prohibido el consumo de alimentos en la sala.</t>
+  </si>
+  <si>
+    <t>piscina001.jpg</t>
+  </si>
+  <si>
+    <t>gimnasio002.jpg</t>
+  </si>
+  <si>
+    <t>piscinaadultos003.jpg</t>
+  </si>
+  <si>
+    <t>salón de eventos004.jpg</t>
+  </si>
+  <si>
+    <t>cancha de fútbol005.jpg</t>
+  </si>
+  <si>
+    <t>piscina pequeña006.jpg</t>
+  </si>
+  <si>
+    <t>zona bbq007.jpg</t>
+  </si>
+  <si>
+    <t>cancha de tenis008.jpg</t>
+  </si>
+  <si>
+    <t>sala de juegos009.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -336,28 +510,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="16"/>
-      <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -417,7 +569,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -439,29 +591,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -823,7 +987,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -839,23 +1003,23 @@
         <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -872,7 +1036,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF3124B0-BF43-4D8E-8B80-2D2432DEB873}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -881,18 +1045,18 @@
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="23.88671875" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="5" max="5" width="25.88671875" customWidth="1"/>
     <col min="6" max="6" width="23.88671875" customWidth="1"/>
-    <col min="7" max="7" width="38.88671875" customWidth="1"/>
+    <col min="7" max="7" width="43.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
@@ -910,7 +1074,7 @@
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -950,14 +1114,14 @@
         <v>3053456459</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" s="12">
-        <v>123456</v>
+        <v>108</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>100</v>
       </c>
       <c r="G4" s="13" t="str">
         <f>B4&amp;"-"&amp;D4&amp;"-"&amp;E4</f>
-        <v>Carlos-3053456459-carlos@gmail.com</v>
+        <v>Carlos-3053456459-carlos@example.com</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -974,13 +1138,13 @@
         <v>3584418688</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" s="1">
-        <v>654321</v>
+        <v>51</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="G5" s="13" t="str">
-        <f t="shared" ref="G5:G6" si="0">B5&amp;"-"&amp;D5&amp;"-"&amp;E5</f>
+        <f t="shared" ref="G5:G9" si="0">B5&amp;"-"&amp;D5&amp;"-"&amp;E5</f>
         <v>Sara-3584418688-sara@gmail.com</v>
       </c>
     </row>
@@ -988,14 +1152,90 @@
       <c r="A6" s="9">
         <v>3</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="B6" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3209876543</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="G6" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>--</v>
+        <v>María -3209876543-maria.gonzalez@example.com</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3156789012</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G7" s="13" t="str">
+        <f>B7&amp;"-"&amp;D7&amp;"-"&amp;E7</f>
+        <v>Laura-3156789012-laura.martinez@example.com</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3007654321</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G8" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>Andrés-3007654321-andres.lopez@example.com</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3182345678</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G9" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>Sofía-3182345678-sofia.torres@example.com</v>
       </c>
     </row>
   </sheetData>
@@ -1007,6 +1247,7 @@
     <hyperlink ref="E5" r:id="rId2" xr:uid="{9C9CCAC3-14F6-486E-9A86-67C2D1CAFF52}"/>
     <hyperlink ref="A1" location="Objetos de dominio!A1" display="Objetos de dominio!A1" xr:uid="{C1ED9137-81DC-43DF-B6AA-ED6EFD23837F}"/>
     <hyperlink ref="A1:D1" location="'Objetos de dominio'!A1" display="&lt;&lt;&lt;&lt;&lt;&lt; Volver al inicio" xr:uid="{C5E3491F-ED23-4E33-A420-E536F5397D68}"/>
+    <hyperlink ref="E7" r:id="rId3" xr:uid="{8AA42C50-8743-4319-B0E5-4D686BB0533B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1014,28 +1255,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CCBB1F3-C6CB-4282-9EE1-3BEE3EA280EE}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="6" width="21.6640625" customWidth="1"/>
-    <col min="7" max="8" width="36" customWidth="1"/>
-    <col min="9" max="9" width="29" customWidth="1"/>
+    <col min="7" max="7" width="36" customWidth="1"/>
+    <col min="8" max="8" width="43.88671875" customWidth="1"/>
+    <col min="9" max="9" width="34.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
@@ -1051,13 +1293,13 @@
         <v>17</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>82</v>
-      </c>
       <c r="F2" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>18</v>
@@ -1078,13 +1320,13 @@
         <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>1</v>
@@ -1107,10 +1349,10 @@
         <v>12</v>
       </c>
       <c r="D4" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>76</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>77</v>
       </c>
       <c r="F4" s="9">
         <v>3053451564</v>
@@ -1118,9 +1360,9 @@
       <c r="G4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="24" t="str">
+      <c r="H4" s="15" t="str">
         <f>Administrador!G4</f>
-        <v>Carlos-3053456459-carlos@gmail.com</v>
+        <v>Carlos-3053456459-carlos@example.com</v>
       </c>
       <c r="I4" s="10" t="str">
         <f>_xlfn.CONCAT(A4,"-",B4)</f>
@@ -1138,10 +1380,10 @@
         <v>45</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F5" s="9">
         <v>3057477789</v>
@@ -1149,13 +1391,106 @@
       <c r="G5" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H5" s="24" t="str">
+      <c r="H5" s="15" t="str">
         <f>Administrador!G5</f>
         <v>Sara-3584418688-sara@gmail.com</v>
       </c>
       <c r="I5" s="10" t="str">
         <f>_xlfn.CONCAT(A5,"-",B5)</f>
         <v>2-Natural</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3001234567</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H6" s="15" t="str">
+        <f>Administrador!G6</f>
+        <v>María -3209876543-maria.gonzalez@example.com</v>
+      </c>
+      <c r="I6" s="10" t="str">
+        <f t="shared" ref="I6:I8" si="0">_xlfn.CONCAT(A6,"-",B6)</f>
+        <v>3-Riogrande</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" s="1">
+        <v>3207654321</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H7" s="15" t="str">
+        <f>Administrador!G7</f>
+        <v>Laura-3156789012-laura.martinez@example.com</v>
+      </c>
+      <c r="I7" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>4-Bolivar</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8" s="1">
+        <v>3109876543</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="H8" s="15" t="str">
+        <f>Administrador!G8</f>
+        <v>Andrés-3007654321-andres.lopez@example.com</v>
+      </c>
+      <c r="I8" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>5-Ventus</v>
       </c>
     </row>
   </sheetData>
@@ -1170,6 +1505,7 @@
     <hyperlink ref="A1:F1" location="'Objetos de dominio'!A1" display="&lt;&lt;&lt;&lt;&lt;&lt; Volver al inicio" xr:uid="{E47C9477-04BF-4359-AA4E-108F5F557D82}"/>
     <hyperlink ref="H3" location="Administrador!A1" display="Administrador" xr:uid="{8573C9AA-E4AB-4C12-80E7-A396F426EDA8}"/>
     <hyperlink ref="H5" location="Administrador!A4" display="Carlos-carlos@gmail.com" xr:uid="{B691C4A3-C438-46E2-9139-486F3E66B20C}"/>
+    <hyperlink ref="H6:H8" location="Administrador!A4" display="Carlos-carlos@gmail.com" xr:uid="{59A54CB4-A9B8-4752-8A52-FC6023395723}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1179,8 +1515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{615584B6-BB9C-4024-AABA-069882FFA83A}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1192,12 +1528,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
       <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1222,10 +1558,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>2</v>
@@ -1239,7 +1575,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -1257,7 +1593,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -1275,7 +1611,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
@@ -1293,7 +1629,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
@@ -1312,12 +1648,12 @@
         <v>5</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="1">
         <v>4</v>
       </c>
-      <c r="D8" s="1" t="str">
+      <c r="D8" s="3" t="str">
         <f>ConjuntoResidencial!I4</f>
         <v>1-Forest apartamentos</v>
       </c>
@@ -1330,58 +1666,86 @@
       <c r="A9" s="1">
         <v>6</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="B9" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3" t="str">
+        <f>ConjuntoResidencial!I6</f>
+        <v>3-Riogrande</v>
+      </c>
       <c r="E9" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> de </v>
+        <v>Bloque2 de 3-Riogrande</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>7</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="B10" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="1">
+        <v>5</v>
+      </c>
+      <c r="D10" s="3" t="str">
+        <f>ConjuntoResidencial!I8</f>
+        <v>5-Ventus</v>
+      </c>
       <c r="E10" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> de </v>
+        <v>Bloque5 de 5-Ventus</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>8</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="B11" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="1">
+        <v>7</v>
+      </c>
+      <c r="D11" s="3" t="str">
+        <f>ConjuntoResidencial!I7</f>
+        <v>4-Bolivar</v>
+      </c>
       <c r="E11" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> de </v>
+        <v>Torre7 de 4-Bolivar</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>9</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="B12" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="1">
+        <v>3</v>
+      </c>
+      <c r="D12" s="3" t="str">
+        <f>ConjuntoResidencial!I6</f>
+        <v>3-Riogrande</v>
+      </c>
       <c r="E12" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> de </v>
+        <v>Bloque3 de 3-Riogrande</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1401,6 +1765,11 @@
     <hyperlink ref="D4" location="ConjuntoResidencial!A4" display="1-Forest apartamentos" xr:uid="{FE6B8B9A-D67F-410F-9E6F-226B627CD379}"/>
     <hyperlink ref="D5:D6" location="ConjuntoResidencial!A4" display="1-Forest apartamentos" xr:uid="{26734694-0972-4ADC-AA89-B0972D85EEB6}"/>
     <hyperlink ref="D7" location="ConjuntoResidencial!A5" display="ConjuntoResidencial!A5" xr:uid="{8C0CBF64-4C4C-4615-84CA-37407A122B1B}"/>
+    <hyperlink ref="D8" location="ConjuntoResidencial!A4" display="ConjuntoResidencial!A4" xr:uid="{424EF75D-3021-4DCE-AC86-B7B197E2AA3F}"/>
+    <hyperlink ref="D9" location="ConjuntoResidencial!A6" display="ConjuntoResidencial!A6" xr:uid="{90A0238A-B68E-43CA-A4E7-622B7D624F49}"/>
+    <hyperlink ref="D10" location="ConjuntoResidencial!A8" display="ConjuntoResidencial!A8" xr:uid="{28B59E02-AAE4-463A-BA1C-AF2FB360623A}"/>
+    <hyperlink ref="D11" location="ConjuntoResidencial!A7" display="ConjuntoResidencial!A7" xr:uid="{466D4C91-E5E2-4912-BD49-0C66AEDD1636}"/>
+    <hyperlink ref="D12" location="ConjuntoResidencial!A6" display="ConjuntoResidencial!A6" xr:uid="{BB64C223-5AFB-4870-A3BB-24CF127D7640}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1411,7 +1780,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1423,12 +1792,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
       <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1453,13 +1822,13 @@
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>8</v>
@@ -1470,7 +1839,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" s="1">
         <v>102</v>
@@ -1489,7 +1858,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" s="1">
         <v>10</v>
@@ -1499,7 +1868,7 @@
         <v>Bloque1 de 1-Forest apartamentos</v>
       </c>
       <c r="E5" s="10" t="str">
-        <f t="shared" ref="E5:E10" si="0">_xlfn.CONCAT(B5," '",C5,"'"," de ",D5)</f>
+        <f t="shared" ref="E5:E13" si="0">_xlfn.CONCAT(B5," '",C5,"'"," de ",D5)</f>
         <v>Casa '10' de Bloque1 de 1-Forest apartamentos</v>
       </c>
     </row>
@@ -1508,7 +1877,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" s="1">
         <v>304</v>
@@ -1527,7 +1896,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C7" s="1">
         <v>11</v>
@@ -1545,46 +1914,124 @@
       <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="B8" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="1">
+        <v>423</v>
+      </c>
+      <c r="D8" s="1" t="str">
+        <f>Zonainmueble!E10</f>
+        <v>Bloque5 de 5-Ventus</v>
+      </c>
       <c r="E8" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> '' de </v>
+        <v>Apartamento '423' de Bloque5 de 5-Ventus</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>6</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="B9" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1204</v>
+      </c>
+      <c r="D9" s="1" t="str">
+        <f>Zonainmueble!E11</f>
+        <v>Torre7 de 4-Bolivar</v>
+      </c>
       <c r="E9" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> '' de </v>
+        <v>Apartamento '1204' de Torre7 de 4-Bolivar</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>7</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="B10" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="1">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1" t="str">
+        <f>Zonainmueble!E7</f>
+        <v>Bloque2 de 2-Natural</v>
+      </c>
       <c r="E10" s="10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> '' de </v>
+        <v>Casa '5' de Bloque2 de 2-Natural</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="9">
+        <v>8</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="19">
+        <v>17</v>
+      </c>
+      <c r="D11" s="1" t="str">
+        <f>Zonainmueble!E12</f>
+        <v>Bloque3 de 3-Riogrande</v>
+      </c>
+      <c r="E11" s="10" t="str">
+        <f>_xlfn.CONCAT(B11," '",C11,"'"," de ",D11)</f>
+        <v>Casa '17' de Bloque3 de 3-Riogrande</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>9</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="19">
+        <v>514</v>
+      </c>
+      <c r="D12" s="1" t="str">
+        <f>Zonainmueble!E9</f>
+        <v>Bloque2 de 3-Riogrande</v>
+      </c>
+      <c r="E12" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>Apartamento '514' de Bloque2 de 3-Riogrande</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>10</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="19">
+        <v>23</v>
+      </c>
+      <c r="D13" s="1" t="str">
+        <f>Zonainmueble!E7</f>
+        <v>Bloque2 de 2-Natural</v>
+      </c>
+      <c r="E13" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>Casa '23' de Bloque2 de 2-Natural</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1611,16 +2058,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F3E3BD9-49ED-471B-BA3A-A84E923CE558}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
     <col min="5" max="7" width="21.6640625" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
@@ -1660,7 +2107,7 @@
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>35</v>
@@ -1686,13 +2133,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>21</v>
@@ -1704,101 +2151,332 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="15">
+    <row r="4" spans="1:10" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="24">
         <v>1</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="17" t="s">
+      <c r="C4" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="24">
         <v>50</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="24">
         <v>60</v>
       </c>
-      <c r="G4" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="H4" s="5" t="s">
+      <c r="G4" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="3" t="str">
+      <c r="I4" s="25" t="str">
         <f>ConjuntoResidencial!$I$4</f>
         <v>1-Forest apartamentos</v>
       </c>
-      <c r="J4" s="10" t="str">
+      <c r="J4" s="26" t="str">
         <f>_xlfn.CONCAT(B4,"-",I4)</f>
         <v>Piscina-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="84" x14ac:dyDescent="0.4">
-      <c r="A5" s="19">
+    <row r="5" spans="1:10" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="27">
         <v>2</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="20" t="s">
+      <c r="C5" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="27">
         <v>20</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="27">
         <v>120</v>
       </c>
-      <c r="G5" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="H5" s="14" t="s">
+      <c r="G5" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="H5" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="3" t="str">
+      <c r="I5" s="25" t="str">
         <f>ConjuntoResidencial!$I$4</f>
         <v>1-Forest apartamentos</v>
       </c>
-      <c r="J5" s="10" t="str">
+      <c r="J5" s="26" t="str">
         <f>_xlfn.CONCAT(B5,"-",I5)</f>
         <v>Gimnasio-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="73.2" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="19">
+    <row r="6" spans="1:10" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="27">
         <v>3</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="22" t="s">
+      <c r="C6" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="27">
         <v>15</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="27">
         <v>1</v>
       </c>
-      <c r="G6" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="H6" s="5" t="s">
+      <c r="G6" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="3" t="str">
+      <c r="I6" s="25" t="str">
         <f>ConjuntoResidencial!$I$5</f>
         <v>2-Natural</v>
       </c>
-      <c r="J6" s="10" t="str">
+      <c r="J6" s="26" t="str">
         <f>_xlfn.CONCAT(B6,"-",I6)</f>
         <v>piscinaAdultos-2-Natural</v>
       </c>
+    </row>
+    <row r="7" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="29">
+        <v>4</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="E7" s="29">
+        <v>100</v>
+      </c>
+      <c r="F7" s="29">
+        <v>4</v>
+      </c>
+      <c r="G7" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="I7" s="25" t="str">
+        <f>ConjuntoResidencial!I6</f>
+        <v>3-Riogrande</v>
+      </c>
+      <c r="J7" s="26" t="str">
+        <f t="shared" ref="J7:J12" si="0">_xlfn.CONCAT(B7,"-",I7)</f>
+        <v>Salón de Eventos-3-Riogrande</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="29">
+        <v>5</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="E8" s="29">
+        <v>22</v>
+      </c>
+      <c r="F8" s="29">
+        <v>90</v>
+      </c>
+      <c r="G8" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="I8" s="25" t="str">
+        <f>ConjuntoResidencial!I7</f>
+        <v>4-Bolivar</v>
+      </c>
+      <c r="J8" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>Cancha de Fútbol-4-Bolivar</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="29">
+        <v>6</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="E9" s="29">
+        <v>20</v>
+      </c>
+      <c r="F9" s="29">
+        <v>45</v>
+      </c>
+      <c r="G9" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="I9" s="25" t="str">
+        <f>ConjuntoResidencial!I5</f>
+        <v>2-Natural</v>
+      </c>
+      <c r="J9" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>Piscina Pequeña-2-Natural</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="29">
+        <v>7</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" s="29">
+        <v>15</v>
+      </c>
+      <c r="F10" s="29">
+        <v>2</v>
+      </c>
+      <c r="G10" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="H10" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="I10" s="25" t="str">
+        <f>ConjuntoResidencial!I8</f>
+        <v>5-Ventus</v>
+      </c>
+      <c r="J10" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>Zona BBQ-5-Ventus</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A11" s="29">
+        <v>8</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="E11" s="29">
+        <v>4</v>
+      </c>
+      <c r="F11" s="29">
+        <v>60</v>
+      </c>
+      <c r="G11" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="I11" s="25" t="str">
+        <f>ConjuntoResidencial!I6</f>
+        <v>3-Riogrande</v>
+      </c>
+      <c r="J11" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>Cancha de Tenis-3-Riogrande</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="29">
+        <v>9</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="E12" s="29">
+        <v>10</v>
+      </c>
+      <c r="F12" s="29">
+        <v>90</v>
+      </c>
+      <c r="G12" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="I12" s="25" t="str">
+        <f>ConjuntoResidencial!I4</f>
+        <v>1-Forest apartamentos</v>
+      </c>
+      <c r="J12" s="26" t="str">
+        <f t="shared" si="0"/>
+        <v>Sala de Juegos-1-Forest apartamentos</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="21"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="17"/>
+      <c r="H13" s="17"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="21"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="17"/>
+      <c r="H14" s="17"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="21"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="17"/>
+      <c r="H15" s="17"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Eliminando muestreo que tenia todas las entidades y contextos
</commit_message>
<xml_diff>
--- a/Doo-Doc/Nueva Version Victus/MuestreoDatos/ConjuntosResidenciales Muestro Datos.xlsx
+++ b/Doo-Doc/Nueva Version Victus/MuestreoDatos/ConjuntosResidenciales Muestro Datos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Music\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\DOO 2024 BD\DOO\victus-doc\Doo-Doc\Nueva Version Victus\MuestreoDatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51CCAB1-80B3-46A6-99AD-F559C35FD6A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D53037-FBB1-4E26-AA7D-9E4BC50D583C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" firstSheet="1" activeTab="5" xr2:uid="{46B52760-6E94-4759-BDEF-A2400BC5A0BB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{46B52760-6E94-4759-BDEF-A2400BC5A0BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Objetos de dominio" sheetId="1" r:id="rId1"/>
@@ -88,9 +88,6 @@
     <t>Es un dato que representa al nombre de un conjunto residencial</t>
   </si>
   <si>
-    <t>Es un dato que representa el formato de texto de una dirección.</t>
-  </si>
-  <si>
     <t>Es un dato que representa la descripción que tiene el conjunto residencial para ser identificado con palabras.</t>
   </si>
   <si>
@@ -238,9 +235,6 @@
     <t>Es un dato que representa el número de contacto de la portería de una conjunto residencial</t>
   </si>
   <si>
-    <t>Es un dato que representa el municipio dónde se encuentra un conjunto residencial.</t>
-  </si>
-  <si>
     <t>Es un dato que representa el departamento dónde se encuentra el conjunto residencial.</t>
   </si>
   <si>
@@ -518,13 +512,19 @@
   </si>
   <si>
     <t>normas</t>
+  </si>
+  <si>
+    <t>Es un dato que representa el formato de texto de una dirección de un conjunto residencial.</t>
+  </si>
+  <si>
+    <t>Es un dato que representa el ciudad dónde se encuentra un conjunto residencial.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -564,6 +564,38 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF4EA72E"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF4EA72E"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -623,7 +655,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -670,6 +702,16 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1012,13 +1054,13 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="2" width="58.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="2" max="2" width="58.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1026,15 +1068,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1042,28 +1084,28 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1086,15 +1128,15 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="23.85546875" customWidth="1"/>
-    <col min="5" max="5" width="25.85546875" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" customWidth="1"/>
-    <col min="7" max="7" width="47.85546875" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" customWidth="1"/>
+    <col min="5" max="5" width="25.88671875" customWidth="1"/>
+    <col min="6" max="6" width="23.88671875" customWidth="1"/>
+    <col min="7" max="7" width="47.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>6</v>
       </c>
@@ -1104,184 +1146,184 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>144</v>
-      </c>
       <c r="G2" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>1</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>41</v>
       </c>
       <c r="D4" s="12">
         <v>3053456459</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G4" s="13" t="str">
         <f>B4&amp;"-"&amp;D4&amp;"-"&amp;E4</f>
         <v>Carlos-3053456459-carlos@example.com</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>2</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>42</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>43</v>
       </c>
       <c r="D5" s="1">
         <v>3584418688</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G5" s="13" t="str">
         <f t="shared" ref="G5:G9" si="0">B5&amp;"-"&amp;D5&amp;"-"&amp;E5</f>
         <v>Sara-3584418688-sara@gmail.com</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>3</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D6" s="1">
         <v>3209876543</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G6" s="13" t="str">
         <f t="shared" si="0"/>
         <v>María -3209876543-maria.gonzalez@example.com</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D7" s="1">
         <v>3156789012</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G7" s="13" t="str">
         <f>B7&amp;"-"&amp;D7&amp;"-"&amp;E7</f>
         <v>Laura-3156789012-laura.martinez@example.com</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D8" s="1">
         <v>3007654321</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G8" s="13" t="str">
         <f t="shared" si="0"/>
         <v>Andrés-3007654321-andres.lopez@example.com</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D9" s="1">
         <v>3182345678</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G9" s="13" t="str">
         <f t="shared" si="0"/>
@@ -1307,19 +1349,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CCBB1F3-C6CB-4282-9EE1-3BEE3EA280EE}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="6" width="21.7109375" customWidth="1"/>
+    <col min="2" max="6" width="21.6640625" customWidth="1"/>
     <col min="7" max="7" width="36" customWidth="1"/>
-    <col min="8" max="8" width="43.85546875" customWidth="1"/>
-    <col min="9" max="9" width="34.28515625" customWidth="1"/>
+    <col min="8" max="8" width="43.88671875" customWidth="1"/>
+    <col min="9" max="9" width="34.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>6</v>
       </c>
@@ -1332,56 +1374,56 @@
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:9" s="28" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H2" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>5</v>
@@ -1390,7 +1432,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -1401,10 +1443,10 @@
         <v>10</v>
       </c>
       <c r="D4" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>61</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>62</v>
       </c>
       <c r="F4" s="9">
         <v>3053451564</v>
@@ -1421,27 +1463,27 @@
         <v>1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>2</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>38</v>
-      </c>
       <c r="D5" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F5" s="9">
         <v>3057477789</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H5" s="15" t="str">
         <f>Administrador!G5</f>
@@ -1452,27 +1494,27 @@
         <v>2-Natural</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F6" s="1">
         <v>3001234567</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H6" s="15" t="str">
         <f>Administrador!G6</f>
@@ -1483,27 +1525,27 @@
         <v>3-Riogrande</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F7" s="1">
         <v>3207654321</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H7" s="15" t="str">
         <f>Administrador!G7</f>
@@ -1514,27 +1556,27 @@
         <v>4-Bolivar</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F8" s="1">
         <v>3109876543</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H8" s="15" t="str">
         <f>Administrador!G8</f>
@@ -1571,15 +1613,15 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" customWidth="1"/>
-    <col min="5" max="5" width="37.140625" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" customWidth="1"/>
+    <col min="5" max="5" width="37.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>6</v>
       </c>
@@ -1588,32 +1630,32 @@
       <c r="D1" s="24"/>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>2</v>
@@ -1622,66 +1664,66 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>1</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4" s="10" t="str">
         <f>_xlfn.CONCAT(B4,C4," de ",D4)</f>
         <v>Torre1 de 1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" s="10" t="str">
         <f t="shared" ref="E5:E12" si="0">_xlfn.CONCAT(B5,C5," de ",D5)</f>
         <v>Bloque1 de 1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6" s="10" t="str">
         <f t="shared" si="0"/>
         <v>Torre2 de 1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>4</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
@@ -1695,12 +1737,12 @@
         <v>Bloque2 de 2-Natural</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>5</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="1">
         <v>4</v>
@@ -1714,12 +1756,12 @@
         <v>Bloque4 de 1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>6</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -1733,12 +1775,12 @@
         <v>Bloque2 de 3-Riogrande</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>7</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="1">
         <v>5</v>
@@ -1752,12 +1794,12 @@
         <v>Bloque5 de 5-Ventus</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>8</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" s="1">
         <v>7</v>
@@ -1771,12 +1813,12 @@
         <v>Torre7 de 4-Bolivar</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>9</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" s="1">
         <v>3</v>
@@ -1825,16 +1867,16 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="31.42578125" customWidth="1"/>
-    <col min="5" max="5" width="49.42578125" customWidth="1"/>
+    <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="31.44140625" customWidth="1"/>
+    <col min="5" max="5" width="49.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>6</v>
       </c>
@@ -1843,46 +1885,46 @@
       <c r="D1" s="24"/>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>133</v>
-      </c>
       <c r="E2" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>1</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="1">
         <v>102</v>
@@ -1896,12 +1938,12 @@
         <v>Apartamento '102' de Torre1 de 1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" s="1">
         <v>10</v>
@@ -1915,12 +1957,12 @@
         <v>Casa '10' de Bloque1 de 1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" s="1">
         <v>304</v>
@@ -1934,12 +1976,12 @@
         <v>Apartamento '304' de Torre2 de 1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>4</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" s="1">
         <v>11</v>
@@ -1953,12 +1995,12 @@
         <v>Casa '11' de Bloque2 de 2-Natural</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>5</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="1">
         <v>423</v>
@@ -1972,12 +2014,12 @@
         <v>Apartamento '423' de Bloque5 de 5-Ventus</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>6</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" s="1">
         <v>1204</v>
@@ -1991,12 +2033,12 @@
         <v>Apartamento '1204' de Torre7 de 4-Bolivar</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>7</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C10" s="1">
         <v>5</v>
@@ -2010,12 +2052,12 @@
         <v>Casa '5' de Bloque2 de 2-Natural</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>8</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C11" s="1">
         <v>17</v>
@@ -2029,12 +2071,12 @@
         <v>Casa '17' de Bloque3 de 3-Riogrande</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>9</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="1">
         <v>514</v>
@@ -2048,12 +2090,12 @@
         <v>Apartamento '514' de Bloque2 de 3-Riogrande</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>10</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C13" s="1">
         <v>23</v>
@@ -2067,14 +2109,14 @@
         <v>Casa '23' de Bloque2 de 2-Natural</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2103,22 +2145,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F3E3BD9-49ED-471B-BA3A-A84E923CE558}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="7" width="21.7109375" customWidth="1"/>
+    <col min="5" max="7" width="21.6640625" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="23.7109375" customWidth="1"/>
-    <col min="10" max="10" width="33.140625" customWidth="1"/>
+    <col min="9" max="9" width="23.6640625" customWidth="1"/>
+    <col min="10" max="10" width="33.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
@@ -2132,62 +2174,62 @@
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="7" t="s">
+    <row r="2" spans="1:10" s="26" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="E2" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="7" t="s">
+      <c r="H2" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J2" s="25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>158</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>2</v>
@@ -2196,7 +2238,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="19">
         <v>1</v>
       </c>
@@ -2204,10 +2246,10 @@
         <v>12</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="19">
         <v>50</v>
@@ -2216,10 +2258,10 @@
         <v>60</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I4" s="20" t="str">
         <f>ConjuntoResidencial!$I$4</f>
@@ -2230,18 +2272,18 @@
         <v>Piscina-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22">
         <v>2</v>
       </c>
       <c r="B5" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" s="23" t="s">
         <v>23</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>24</v>
       </c>
       <c r="E5" s="22">
         <v>20</v>
@@ -2250,10 +2292,10 @@
         <v>120</v>
       </c>
       <c r="G5" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I5" s="20" t="str">
         <f>ConjuntoResidencial!$I$4</f>
@@ -2264,18 +2306,18 @@
         <v>Gimnasio-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="22">
         <v>3</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6" s="22">
         <v>15</v>
@@ -2284,10 +2326,10 @@
         <v>1</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I6" s="20" t="str">
         <f>ConjuntoResidencial!$I$5</f>
@@ -2298,18 +2340,18 @@
         <v>piscinaAdultos-2-Natural</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="22">
         <v>4</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E7" s="22">
         <v>100</v>
@@ -2318,10 +2360,10 @@
         <v>4</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H7" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I7" s="20" t="str">
         <f>ConjuntoResidencial!I6</f>
@@ -2332,18 +2374,18 @@
         <v>Salón de Eventos-3-Riogrande</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A8" s="22">
         <v>5</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E8" s="22">
         <v>22</v>
@@ -2352,10 +2394,10 @@
         <v>90</v>
       </c>
       <c r="G8" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H8" s="23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I8" s="20" t="str">
         <f>ConjuntoResidencial!I7</f>
@@ -2366,18 +2408,18 @@
         <v>Cancha de Fútbol-4-Bolivar</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="22">
         <v>6</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E9" s="22">
         <v>20</v>
@@ -2386,10 +2428,10 @@
         <v>45</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H9" s="23" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I9" s="20" t="str">
         <f>ConjuntoResidencial!I5</f>
@@ -2400,18 +2442,18 @@
         <v>Piscina Pequeña-2-Natural</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="22">
         <v>7</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E10" s="22">
         <v>15</v>
@@ -2420,10 +2462,10 @@
         <v>2</v>
       </c>
       <c r="G10" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H10" s="23" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I10" s="20" t="str">
         <f>ConjuntoResidencial!I8</f>
@@ -2434,18 +2476,18 @@
         <v>Zona BBQ-5-Ventus</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="22">
         <v>8</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E11" s="22">
         <v>4</v>
@@ -2454,10 +2496,10 @@
         <v>60</v>
       </c>
       <c r="G11" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H11" s="23" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I11" s="20" t="str">
         <f>ConjuntoResidencial!I6</f>
@@ -2468,18 +2510,18 @@
         <v>Cancha de Tenis-3-Riogrande</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A12" s="22">
         <v>9</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E12" s="22">
         <v>10</v>
@@ -2488,10 +2530,10 @@
         <v>90</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H12" s="23" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I12" s="20" t="str">
         <f>ConjuntoResidencial!I4</f>
@@ -2502,18 +2544,18 @@
         <v>Sala de Juegos-1-Forest apartamentos</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="18"/>
       <c r="C13" s="17"/>
       <c r="D13" s="16"/>
       <c r="H13" s="16"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C14" s="17"/>
       <c r="D14" s="16"/>
       <c r="H14" s="16"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C15" s="17"/>
       <c r="D15" s="16"/>
       <c r="H15" s="16"/>

</xml_diff>

<commit_message>
Revision y mejora del muestro de datos y modelo anemico de conjuntos residenciales, entidades Zona común,inmueble,administrador,zona inmuebley conjunto residencial
</commit_message>
<xml_diff>
--- a/Doo-Doc/Nueva Version Victus/MuestreoDatos/ConjuntosResidenciales Muestro Datos.xlsx
+++ b/Doo-Doc/Nueva Version Victus/MuestreoDatos/ConjuntosResidenciales Muestro Datos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\DOO 2024 BD\DOO\victus-doc\Doo-Doc\Nueva Version Victus\MuestreoDatos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josez\Documents\Universidad IngeSistemas\Diseño Orientado a Objetos(DOO)\VictusProyect\victus-doc\Doo-Doc\Nueva Version Victus\MuestreoDatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969333AD-F420-4B20-BC89-76A62CB31238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F148B6-2CD6-4E41-88DD-F5BEDF6EFCEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{46B52760-6E94-4759-BDEF-A2400BC5A0BB}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="9132" windowHeight="12336" firstSheet="5" activeTab="5" xr2:uid="{46B52760-6E94-4759-BDEF-A2400BC5A0BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Objetos de dominio" sheetId="1" r:id="rId1"/>
@@ -457,9 +457,6 @@
     <t>contactoRecepcion</t>
   </si>
   <si>
-    <t>Es un dato que representa el número de contacto de una recepcion de un conjunto residencial</t>
-  </si>
-  <si>
     <t>Es un dato que representa la descripción general que tiene el conjunto residencial .</t>
   </si>
   <si>
@@ -539,6 +536,9 @@
   </si>
   <si>
     <t>Este es le dato que representa el tiempo de uso por numero entero de un residente</t>
+  </si>
+  <si>
+    <t>Es un dato que representa el numero de contacto de la recepción del conjunto residencial.</t>
   </si>
 </sst>
 </file>
@@ -735,16 +735,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -760,6 +757,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1153,7 +1153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3601F120-B689-4608-A7AB-FD2F4140FEAD}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -1232,8 +1232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF3124B0-BF43-4D8E-8B80-2D2432DEB873}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1252,50 +1252,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:11" s="30" customFormat="1" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+    <row r="2" spans="1:11" s="29" customFormat="1" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="E2" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="E2" s="28" t="s">
-        <v>150</v>
-      </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="J2" s="27" t="s">
         <v>152</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="K2" s="27" t="s">
         <v>153</v>
-      </c>
-      <c r="K2" s="28" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -1309,16 +1309,16 @@
         <v>127</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="F3" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>142</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>30</v>
@@ -1327,10 +1327,10 @@
         <v>7</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -1344,7 +1344,7 @@
         <v>35</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E4" s="8">
         <v>1017245136</v>
@@ -1382,7 +1382,7 @@
         <v>37</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E5" s="8">
         <v>5987645832</v>
@@ -1397,7 +1397,7 @@
         <v>71</v>
       </c>
       <c r="I5" s="12" t="str">
-        <f t="shared" ref="I5:K9" si="0">D5&amp;"-"&amp;E5</f>
+        <f t="shared" ref="I5:I9" si="0">D5&amp;"-"&amp;E5</f>
         <v>cedula-5987645832</v>
       </c>
       <c r="J5" s="12">
@@ -1420,7 +1420,7 @@
         <v>68</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E6" s="8">
         <v>8574693214</v>
@@ -1458,7 +1458,7 @@
         <v>74</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E7" s="1">
         <v>5789687456</v>
@@ -1496,7 +1496,7 @@
         <v>78</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E8" s="1">
         <v>1112587693</v>
@@ -1534,7 +1534,7 @@
         <v>82</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E9" s="1">
         <v>8574693218</v>
@@ -1580,8 +1580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CCBB1F3-C6CB-4282-9EE1-3BEE3EA280EE}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView topLeftCell="I2" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1594,81 +1594,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="1:10" s="29" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+    <row r="2" spans="1:10" s="28" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="G2" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="H2" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="26" t="s">
         <v>138</v>
-      </c>
-      <c r="H2" s="28" t="s">
-        <v>121</v>
-      </c>
-      <c r="I2" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="28" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="F3" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="G3" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="H3" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="27" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -1733,7 +1733,7 @@
         <v>cedula-5987645832</v>
       </c>
       <c r="I5" s="9" t="str">
-        <f t="shared" ref="I5:J8" si="0">_xlfn.CONCAT(B5)</f>
+        <f t="shared" ref="I5:I8" si="0">_xlfn.CONCAT(B5)</f>
         <v>Natural</v>
       </c>
       <c r="J5" s="9">
@@ -1869,8 +1869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{615584B6-BB9C-4024-AABA-069882FFA83A}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1882,29 +1882,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" s="31" customFormat="1" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+    <row r="2" spans="1:5" s="30" customFormat="1" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="E2" s="28" t="s">
-        <v>155</v>
+      <c r="E2" s="27" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1931,7 +1931,7 @@
       <c r="B4" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="32">
+      <c r="C4" s="31">
         <v>1</v>
       </c>
       <c r="D4" s="3" t="str">
@@ -1950,7 +1950,7 @@
       <c r="B5" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="32">
+      <c r="C5" s="31">
         <v>1</v>
       </c>
       <c r="D5" s="3" t="str">
@@ -1969,7 +1969,7 @@
       <c r="B6" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="32">
+      <c r="C6" s="31">
         <v>2</v>
       </c>
       <c r="D6" s="3" t="str">
@@ -1988,7 +1988,7 @@
       <c r="B7" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="31">
         <v>1</v>
       </c>
       <c r="D7" s="3" t="str">
@@ -2007,7 +2007,7 @@
       <c r="B8" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="31">
         <v>1</v>
       </c>
       <c r="D8" s="3" t="str">
@@ -2026,7 +2026,7 @@
       <c r="B9" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="32">
+      <c r="C9" s="31">
         <v>1</v>
       </c>
       <c r="D9" s="3" t="str">
@@ -2045,7 +2045,7 @@
       <c r="B10" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="31">
         <v>1</v>
       </c>
       <c r="D10" s="3" t="str">
@@ -2064,7 +2064,7 @@
       <c r="B11" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="32">
+      <c r="C11" s="31">
         <v>1</v>
       </c>
       <c r="D11" s="3" t="str">
@@ -2083,7 +2083,7 @@
       <c r="B12" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="32">
+      <c r="C12" s="31">
         <v>2</v>
       </c>
       <c r="D12" s="3" t="str">
@@ -2126,8 +2126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{488BF9E0-DC4F-43E4-93DE-0EE5B6337FDE}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2140,29 +2140,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
       <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" s="27" t="s">
         <v>157</v>
-      </c>
-      <c r="D2" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="E2" s="28" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -2173,7 +2173,7 @@
         <v>45</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>43</v>
@@ -2183,7 +2183,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="33">
+      <c r="A4" s="32">
         <v>1</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -2202,7 +2202,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="32">
+      <c r="A5" s="31">
         <v>2</v>
       </c>
       <c r="B5" s="8" t="s">
@@ -2221,7 +2221,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="32">
+      <c r="A6" s="31">
         <v>3</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -2240,7 +2240,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="32">
+      <c r="A7" s="31">
         <v>4</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -2259,7 +2259,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="32">
+      <c r="A8" s="31">
         <v>5</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -2278,7 +2278,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="32">
+      <c r="A9" s="31">
         <v>6</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -2297,7 +2297,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="32">
+      <c r="A10" s="31">
         <v>7</v>
       </c>
       <c r="B10" s="8" t="s">
@@ -2316,7 +2316,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="33">
+      <c r="A11" s="32">
         <v>8</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -2335,7 +2335,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="32">
+      <c r="A12" s="31">
         <v>9</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -2354,7 +2354,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="32">
+      <c r="A13" s="31">
         <v>10</v>
       </c>
       <c r="B13" s="8" t="s">
@@ -2404,8 +2404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F3E3BD9-49ED-471B-BA3A-A84E923CE558}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2434,7 +2434,7 @@
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="1:10" s="34" customFormat="1" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="33" customFormat="1" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>26</v>
       </c>
@@ -2451,10 +2451,10 @@
         <v>23</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H2" s="23" t="s">
         <v>24</v>
@@ -2474,19 +2474,19 @@
         <v>126</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>132</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>133</v>
@@ -2600,7 +2600,7 @@
         <v>piscinaAdultos-Natural</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="21">
         <v>4</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>Salón de Eventos-Riogrande</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="21">
         <v>5</v>
       </c>
@@ -2668,7 +2668,7 @@
         <v>Cancha de Fútbol-Bolivar</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="21">
         <v>6</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>Piscina Pequeña-Natural</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="21">
         <v>7</v>
       </c>
@@ -2736,7 +2736,7 @@
         <v>Zona BBQ-Ventus</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="21">
         <v>8</v>
       </c>
@@ -2770,7 +2770,7 @@
         <v>Cancha de Tenis-Riogrande</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="21">
         <v>9</v>
       </c>

</xml_diff>